<commit_message>
linear regression attempt 1
</commit_message>
<xml_diff>
--- a/data/Cleaned_Data.xlsx
+++ b/data/Cleaned_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holde\_Villanova\Junior Spring\Machine-Learning\_final_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBC08DB-0518-4604-84FD-AD220890D394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74359656-51EB-46A7-96FD-8F7403F351D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="9" xr2:uid="{AB9AB9B0-C27F-4564-94E8-73F2C94166A3}"/>
+    <workbookView xWindow="547" yWindow="0" windowWidth="25133" windowHeight="13593" activeTab="1" xr2:uid="{AB9AB9B0-C27F-4564-94E8-73F2C94166A3}"/>
   </bookViews>
   <sheets>
     <sheet name="NOW-US" sheetId="2" r:id="rId1"/>
@@ -747,7 +747,7 @@
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:K1"/>
+      <selection activeCell="A2" sqref="A2:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.4"/>
@@ -1995,8 +1995,8 @@
   </sheetPr>
   <dimension ref="A1:AO16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.4"/>
@@ -3913,8 +3913,8 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.4"/>
@@ -4737,7 +4737,7 @@
   <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.4"/>
@@ -7532,7 +7532,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.4"/>

</xml_diff>